<commit_message>
Added test case that requires more than one set of data
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/swagLabsData.xlsx
+++ b/src/test/resources/testData/swagLabsData.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://planittesting-my.sharepoint.com/personal/ryadav_planittesting_com/Documents/Desktop/Playwright_Automation_Framework/src/test/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{D1D58FCC-BEE9-4441-94AB-35ACA6EFA77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7335166D-BA53-4FAD-85F8-2B22BCE28606}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="8_{D1D58FCC-BEE9-4441-94AB-35ACA6EFA77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07D93382-64CD-49E9-9082-8763F2CC5612}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6512A4E0-8F70-4115-B37D-5A43B970B6F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{6512A4E0-8F70-4115-B37D-5A43B970B6F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Cart Details" sheetId="2" r:id="rId2"/>
+    <sheet name="Contact Details" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>username</t>
   </si>
@@ -69,6 +71,42 @@
   </si>
   <si>
     <t>invalid</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Sauce Labs Backpack</t>
+  </si>
+  <si>
+    <t>Test.allTheThings() T-Shirt (Red)</t>
+  </si>
+  <si>
+    <t>Sauce Labs Fleece Jacket</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Ronak</t>
+  </si>
+  <si>
+    <t>Yadav</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>Demo Last Name</t>
   </si>
 </sst>
 </file>
@@ -90,7 +128,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,8 +141,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -127,15 +171,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -151,6 +215,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -472,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE91DAC-20DE-42F7-BD07-79DAA03B3470}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -563,4 +631,102 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6777F16-B25E-443B-B499-A6D857B6D2C5}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF1E76B-2587-47A6-B667-D17A1680E00F}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="5">
+        <v>401209</v>
+      </c>
+      <c r="D2" s="5">
+        <v>103.65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="6">
+        <v>401210</v>
+      </c>
+      <c r="D3" s="6">
+        <v>103.65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
26/11/2025 commit with some changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/swagLabsData.xlsx
+++ b/src/test/resources/testData/swagLabsData.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="144" documentId="8_{D1D58FCC-BEE9-4441-94AB-35ACA6EFA77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07D93382-64CD-49E9-9082-8763F2CC5612}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{6512A4E0-8F70-4115-B37D-5A43B970B6F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6512A4E0-8F70-4115-B37D-5A43B970B6F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -215,10 +215,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -540,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE91DAC-20DE-42F7-BD07-79DAA03B3470}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
@@ -637,7 +633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6777F16-B25E-443B-B499-A6D857B6D2C5}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -676,7 +672,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>